<commit_message>
Update Bit_Geekss_Contribution  (KHANT TI KYI).xlsx
</commit_message>
<xml_diff>
--- a/Bit Geeks - Project/Bit_Geekss_Contribution  (KHANT TI KYI).xlsx
+++ b/Bit Geeks - Project/Bit_Geekss_Contribution  (KHANT TI KYI).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bit-Geek-Project-Documents-\Bit Geeks - Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605C9908-B5DE-4E16-AC3D-8C02B39A9F3B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD2075-0287-43C4-8700-C14A9B527F3E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="37">
   <si>
     <t>Attendance</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Yune Nandi Oo</t>
+  </si>
+  <si>
+    <t>CT6008</t>
   </si>
 </sst>
 </file>
@@ -322,6 +325,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -331,9 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,6 +866,156 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1783080</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF6649E5-39A5-42E2-B8B5-B5A3BB89E1A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4747260" y="3543300"/>
+          <a:ext cx="2446020" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Determine the project</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> scope and timeline. Discuss the system requirements and determine programming languages.Gather the requirement of the system of the app with team members. And specify the role and responibilities of each members. Test the whole system of the applicatoin with Gone Sin Mal  specification. And help to solve the problems of the team members with their difficulty  Editing the video trailer of Gone-Sin-Mal app. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1805940</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24070BF9-0AAA-4D81-9C5B-DD6CC8D5AD37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4640580" y="8526780"/>
+          <a:ext cx="2575560" cy="2994660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Develop the Gone Sin Mal backend with</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> react native. Discuss the Design(UI) with frontend team members and fix the bug or errors of the programs not only his responbilities but also help the team members.  Moreover he is the director of the video trailer of Gone Sin Mal app.  </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1192,8 +1345,8 @@
   </sheetPr>
   <dimension ref="A1:T149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,26 +1379,28 @@
       <c r="O1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="4"/>
+      <c r="Q1" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
       <c r="O3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1277,19 +1432,19 @@
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
       <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1313,18 +1468,18 @@
         <v>14</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
       <c r="M7" s="6"/>
       <c r="O7" s="11" t="s">
         <v>15</v>
@@ -1352,7 +1507,7 @@
       <c r="G10">
         <v>3</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="19">
         <v>4</v>
       </c>
       <c r="K10">
@@ -1375,7 +1530,7 @@
       <c r="G11">
         <v>3</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="19">
         <v>4</v>
       </c>
       <c r="K11">
@@ -1455,7 +1610,7 @@
       <c r="C17" s="4"/>
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="I17" s="23"/>
+      <c r="I17" s="20"/>
       <c r="K17" s="4"/>
       <c r="M17" s="4"/>
       <c r="O17" s="12"/>
@@ -1495,8 +1650,8 @@
       <c r="C20" s="4"/>
       <c r="E20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="I20" s="24"/>
-      <c r="K20" s="23"/>
+      <c r="I20" s="21"/>
+      <c r="K20" s="20"/>
       <c r="M20" s="4"/>
       <c r="O20" s="12"/>
     </row>
@@ -1534,8 +1689,8 @@
       </c>
       <c r="C23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="G23" s="24"/>
-      <c r="I23" s="23"/>
+      <c r="G23" s="21"/>
+      <c r="I23" s="20"/>
       <c r="K23" s="4"/>
       <c r="M23" s="4"/>
       <c r="O23" s="12"/>
@@ -1575,7 +1730,7 @@
       </c>
       <c r="C26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="20"/>
       <c r="I26" s="4"/>
       <c r="K26" s="4"/>
       <c r="M26" s="4"/>
@@ -1616,7 +1771,7 @@
       <c r="C29" s="4"/>
       <c r="E29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="I29" s="23"/>
+      <c r="I29" s="20"/>
       <c r="K29" s="4"/>
       <c r="M29" s="4"/>
       <c r="O29" s="12"/>
@@ -1675,19 +1830,19 @@
       <c r="A34" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="21"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="24"/>
       <c r="O34" s="13" t="s">
         <v>25</v>
       </c>
@@ -1721,7 +1876,7 @@
       <c r="E36" s="4"/>
       <c r="G36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="K36" s="23"/>
+      <c r="K36" s="20"/>
       <c r="M36" s="4"/>
       <c r="O36" s="12"/>
     </row>
@@ -1761,7 +1916,7 @@
       <c r="E39" s="4"/>
       <c r="G39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="K39" s="23"/>
+      <c r="K39" s="20"/>
       <c r="M39" s="4"/>
       <c r="O39" s="12"/>
     </row>
@@ -1801,7 +1956,7 @@
       <c r="E42" s="4"/>
       <c r="G42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="K42" s="23"/>
+      <c r="K42" s="20"/>
       <c r="M42" s="4"/>
       <c r="O42" s="12"/>
     </row>
@@ -1841,7 +1996,7 @@
       <c r="E45" s="4"/>
       <c r="G45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="K45" s="23"/>
+      <c r="K45" s="20"/>
       <c r="M45" s="4"/>
       <c r="O45" s="12"/>
     </row>
@@ -1881,7 +2036,7 @@
       <c r="E48" s="4"/>
       <c r="G48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="K48" s="23"/>
+      <c r="K48" s="20"/>
       <c r="M48" s="4"/>
       <c r="O48" s="12"/>
     </row>
@@ -1908,19 +2063,19 @@
       <c r="A55" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="20"/>
-      <c r="M55" s="21"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="24"/>
       <c r="O55" s="13" t="s">
         <v>25</v>
       </c>
@@ -1954,7 +2109,7 @@
       <c r="E57" s="4"/>
       <c r="G57" s="4"/>
       <c r="I57" s="4"/>
-      <c r="K57" s="23"/>
+      <c r="K57" s="20"/>
       <c r="M57" s="4"/>
       <c r="O57" s="12"/>
     </row>
@@ -1994,7 +2149,7 @@
       <c r="E60" s="4"/>
       <c r="G60" s="4"/>
       <c r="I60" s="4"/>
-      <c r="K60" s="23"/>
+      <c r="K60" s="20"/>
       <c r="M60" s="4"/>
       <c r="O60" s="12"/>
     </row>
@@ -2034,7 +2189,7 @@
       <c r="E63" s="4"/>
       <c r="G63" s="4"/>
       <c r="I63" s="4"/>
-      <c r="K63" s="23"/>
+      <c r="K63" s="20"/>
       <c r="M63" s="4"/>
       <c r="O63" s="12"/>
     </row>
@@ -2074,7 +2229,7 @@
       <c r="E66" s="4"/>
       <c r="G66" s="4"/>
       <c r="I66" s="4"/>
-      <c r="K66" s="23"/>
+      <c r="K66" s="20"/>
       <c r="M66" s="4"/>
       <c r="O66" s="12"/>
     </row>
@@ -2114,7 +2269,7 @@
       <c r="E69" s="4"/>
       <c r="G69" s="4"/>
       <c r="I69" s="4"/>
-      <c r="K69" s="23"/>
+      <c r="K69" s="20"/>
       <c r="M69" s="4"/>
       <c r="O69" s="12"/>
     </row>
@@ -2234,19 +2389,19 @@
       <c r="A89" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="20"/>
-      <c r="H89" s="20"/>
-      <c r="I89" s="20"/>
-      <c r="J89" s="20"/>
-      <c r="K89" s="20"/>
-      <c r="L89" s="20"/>
-      <c r="M89" s="21"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="24"/>
       <c r="O89" s="13" t="s">
         <v>25</v>
       </c>
@@ -2280,7 +2435,7 @@
       <c r="E91" s="4"/>
       <c r="G91" s="4"/>
       <c r="I91" s="4"/>
-      <c r="K91" s="23"/>
+      <c r="K91" s="20"/>
       <c r="M91" s="4"/>
       <c r="O91" s="12"/>
     </row>
@@ -2320,7 +2475,7 @@
       <c r="E94" s="4"/>
       <c r="G94" s="4"/>
       <c r="I94" s="4"/>
-      <c r="K94" s="23"/>
+      <c r="K94" s="20"/>
       <c r="M94" s="4"/>
       <c r="O94" s="12"/>
     </row>
@@ -2359,7 +2514,7 @@
       <c r="C97" s="4"/>
       <c r="E97" s="4"/>
       <c r="G97" s="4"/>
-      <c r="I97" s="23"/>
+      <c r="I97" s="20"/>
       <c r="K97" s="4"/>
       <c r="M97" s="4"/>
       <c r="O97" s="12"/>
@@ -2399,7 +2554,7 @@
       <c r="C100" s="4"/>
       <c r="E100" s="4"/>
       <c r="G100" s="4"/>
-      <c r="I100" s="23"/>
+      <c r="I100" s="20"/>
       <c r="K100" s="4"/>
       <c r="M100" s="4"/>
       <c r="O100" s="12"/>
@@ -2439,7 +2594,7 @@
       <c r="C103" s="4"/>
       <c r="E103" s="4"/>
       <c r="G103" s="4"/>
-      <c r="I103" s="23"/>
+      <c r="I103" s="20"/>
       <c r="K103" s="4"/>
       <c r="M103" s="4"/>
       <c r="O103" s="12"/>
@@ -2473,19 +2628,19 @@
       <c r="A113" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C113" s="19" t="s">
+      <c r="C113" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="20"/>
-      <c r="H113" s="20"/>
-      <c r="I113" s="20"/>
-      <c r="J113" s="20"/>
-      <c r="K113" s="20"/>
-      <c r="L113" s="20"/>
-      <c r="M113" s="21"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="23"/>
+      <c r="H113" s="23"/>
+      <c r="I113" s="23"/>
+      <c r="J113" s="23"/>
+      <c r="K113" s="23"/>
+      <c r="L113" s="23"/>
+      <c r="M113" s="24"/>
       <c r="O113" s="13" t="s">
         <v>25</v>
       </c>
@@ -2518,7 +2673,7 @@
       <c r="C115" s="4"/>
       <c r="E115" s="4"/>
       <c r="G115" s="4"/>
-      <c r="I115" s="23"/>
+      <c r="I115" s="20"/>
       <c r="K115" s="4"/>
       <c r="M115" s="4"/>
       <c r="O115" s="12"/>
@@ -2558,7 +2713,7 @@
       <c r="C118" s="4"/>
       <c r="E118" s="4"/>
       <c r="G118" s="4"/>
-      <c r="I118" s="23"/>
+      <c r="I118" s="20"/>
       <c r="K118" s="4"/>
       <c r="M118" s="4"/>
       <c r="O118" s="12"/>
@@ -2597,7 +2752,7 @@
       </c>
       <c r="C121" s="4"/>
       <c r="E121" s="4"/>
-      <c r="G121" s="23"/>
+      <c r="G121" s="20"/>
       <c r="I121" s="4"/>
       <c r="K121" s="4"/>
       <c r="M121" s="4"/>
@@ -2637,7 +2792,7 @@
       </c>
       <c r="C124" s="4"/>
       <c r="E124" s="4"/>
-      <c r="G124" s="23"/>
+      <c r="G124" s="20"/>
       <c r="I124" s="4"/>
       <c r="K124" s="4"/>
       <c r="M124" s="4"/>
@@ -2677,7 +2832,7 @@
       </c>
       <c r="C127" s="4"/>
       <c r="E127" s="4"/>
-      <c r="G127" s="23"/>
+      <c r="G127" s="20"/>
       <c r="I127" s="4"/>
       <c r="K127" s="4"/>
       <c r="M127" s="4"/>
@@ -2760,19 +2915,19 @@
       <c r="A134" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C134" s="19" t="s">
+      <c r="C134" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D134" s="20"/>
-      <c r="E134" s="20"/>
-      <c r="F134" s="20"/>
-      <c r="G134" s="20"/>
-      <c r="H134" s="20"/>
-      <c r="I134" s="20"/>
-      <c r="J134" s="20"/>
-      <c r="K134" s="20"/>
-      <c r="L134" s="20"/>
-      <c r="M134" s="21"/>
+      <c r="D134" s="23"/>
+      <c r="E134" s="23"/>
+      <c r="F134" s="23"/>
+      <c r="G134" s="23"/>
+      <c r="H134" s="23"/>
+      <c r="I134" s="23"/>
+      <c r="J134" s="23"/>
+      <c r="K134" s="23"/>
+      <c r="L134" s="23"/>
+      <c r="M134" s="24"/>
       <c r="O134" s="13" t="s">
         <v>25</v>
       </c>
@@ -2804,7 +2959,7 @@
       </c>
       <c r="C136" s="4"/>
       <c r="E136" s="4"/>
-      <c r="G136" s="23"/>
+      <c r="G136" s="20"/>
       <c r="I136" s="4"/>
       <c r="K136" s="4"/>
       <c r="M136" s="4"/>
@@ -2844,7 +2999,7 @@
       </c>
       <c r="C139" s="4"/>
       <c r="E139" s="4"/>
-      <c r="G139" s="23"/>
+      <c r="G139" s="20"/>
       <c r="I139" s="4"/>
       <c r="K139" s="4"/>
       <c r="M139" s="4"/>
@@ -2883,7 +3038,7 @@
         <v>7</v>
       </c>
       <c r="C142" s="4"/>
-      <c r="E142" s="23"/>
+      <c r="E142" s="20"/>
       <c r="G142" s="4"/>
       <c r="I142" s="4"/>
       <c r="K142" s="4"/>
@@ -2923,7 +3078,7 @@
         <v>9</v>
       </c>
       <c r="C145" s="4"/>
-      <c r="E145" s="23"/>
+      <c r="E145" s="20"/>
       <c r="G145" s="4"/>
       <c r="I145" s="4"/>
       <c r="K145" s="4"/>
@@ -2963,7 +3118,7 @@
         <v>11</v>
       </c>
       <c r="C148" s="4"/>
-      <c r="E148" s="23"/>
+      <c r="E148" s="20"/>
       <c r="G148" s="4"/>
       <c r="I148" s="4"/>
       <c r="K148" s="4"/>

</xml_diff>